<commit_message>
New testcases for running with Nadia + report + previous results + writing results in a text file
</commit_message>
<xml_diff>
--- a/Algorithm/Test results/tests version 3.xlsx
+++ b/Algorithm/Test results/tests version 3.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="14">
   <si>
     <t xml:space="preserve">Testcase: 0 </t>
   </si>
@@ -150,12 +150,9 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
+                  <a:schemeClr val="tx2"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -183,12 +180,9 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
+                <a:schemeClr val="tx2"/>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
               <a:ea typeface="+mn-ea"/>
@@ -203,7 +197,8 @@
     <c:view3D>
       <c:rotX val="15"/>
       <c:rotY val="20"/>
-      <c:rAngAx val="0"/>
+      <c:depthPercent val="100"/>
+      <c:rAngAx val="1"/>
     </c:view3D>
     <c:floor>
       <c:thickness val="0"/>
@@ -259,9 +254,32 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent2"/>
-            </a:solidFill>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent2">
+                    <a:satMod val="103000"/>
+                    <a:lumMod val="102000"/>
+                    <a:tint val="94000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent2">
+                    <a:satMod val="110000"/>
+                    <a:lumMod val="100000"/>
+                    <a:shade val="100000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent2">
+                    <a:lumMod val="99000"/>
+                    <a:satMod val="120000"/>
+                    <a:shade val="78000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -333,9 +351,32 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent3"/>
-            </a:solidFill>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent3">
+                    <a:satMod val="103000"/>
+                    <a:lumMod val="102000"/>
+                    <a:tint val="94000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent3">
+                    <a:satMod val="110000"/>
+                    <a:lumMod val="100000"/>
+                    <a:shade val="100000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent3">
+                    <a:lumMod val="99000"/>
+                    <a:satMod val="120000"/>
+                    <a:shade val="78000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -407,9 +448,32 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent4"/>
-            </a:solidFill>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent4">
+                    <a:satMod val="103000"/>
+                    <a:lumMod val="102000"/>
+                    <a:tint val="94000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent4">
+                    <a:satMod val="110000"/>
+                    <a:lumMod val="100000"/>
+                    <a:shade val="100000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent4">
+                    <a:lumMod val="99000"/>
+                    <a:satMod val="120000"/>
+                    <a:shade val="78000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -481,9 +545,32 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent5"/>
-            </a:solidFill>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent5">
+                    <a:satMod val="103000"/>
+                    <a:lumMod val="102000"/>
+                    <a:tint val="94000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent5">
+                    <a:satMod val="110000"/>
+                    <a:lumMod val="100000"/>
+                    <a:shade val="100000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent5">
+                    <a:lumMod val="99000"/>
+                    <a:satMod val="120000"/>
+                    <a:shade val="78000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -555,9 +642,32 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent6"/>
-            </a:solidFill>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent6">
+                    <a:satMod val="103000"/>
+                    <a:lumMod val="102000"/>
+                    <a:tint val="94000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent6">
+                    <a:satMod val="110000"/>
+                    <a:lumMod val="100000"/>
+                    <a:shade val="100000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent6">
+                    <a:lumMod val="99000"/>
+                    <a:satMod val="120000"/>
+                    <a:shade val="78000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -622,14 +732,14 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="219"/>
+        <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="108616208"/>
-        <c:axId val="162034368"/>
+        <c:axId val="208936944"/>
+        <c:axId val="208937504"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="108616208"/>
+        <c:axId val="208936944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -642,12 +752,9 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
+                      <a:schemeClr val="tx2"/>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -656,13 +763,8 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="fr-FR"/>
-                  <a:t>Number</a:t>
+                  <a:t>Number of concrete services</a:t>
                 </a:r>
-                <a:r>
-                  <a:rPr lang="fr-FR" baseline="0"/>
-                  <a:t> of concrete services</a:t>
-                </a:r>
-                <a:endParaRPr lang="fr-FR"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -680,12 +782,9 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
+                    <a:schemeClr val="tx2"/>
                   </a:solidFill>
                   <a:latin typeface="+mn-lt"/>
                   <a:ea typeface="+mn-ea"/>
@@ -696,6 +795,479 @@
             </a:p>
           </c:txPr>
         </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx2">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx2"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="208937504"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="208937504"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx2">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx2"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="fr-FR"/>
+                  <a:t>Time</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx2"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="fr-FR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx2"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="208936944"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx2"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx2">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="fr-FR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="pt-BR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="fr-FR"/>
+              <a:t>Experiment 2</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Plan1!$E$27</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Test 1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Plan1!$D$28:$D$33</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Plan1!$E$28:$E$33</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1.2012077000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.6364169</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.2868402999999997</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>13.884088999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>28.501382700000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>54.678350500000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Plan1!$F$27</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Test 2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Plan1!$D$28:$D$33</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Plan1!$F$28:$F$33</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.40560259999999998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.624004</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.5428163000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.8532247000000002</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.0980454999999996</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>20.482931300000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="230883968"/>
+        <c:axId val="226168512"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="230883968"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -733,7 +1305,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="162034368"/>
+        <c:crossAx val="226168512"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -741,7 +1313,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="162034368"/>
+        <c:axId val="226168512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -761,62 +1333,6 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="fr-FR"/>
-                  <a:t>Time</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout/>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="fr-FR"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -848,7 +1364,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="108616208"/>
+        <c:crossAx val="230883968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -893,7 +1409,439 @@
       </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="zero"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="fr-FR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="pt-BR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="fr-FR"/>
+              <a:t>Experiment 3</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Plan1!$E$35</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Test 1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Plan1!$D$36:$D$41</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Plan1!$E$36:$E$41</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>327680</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>990000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2488320</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5493488</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>11010048</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>20470320</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Plan1!$F$35</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Test 2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Plan1!$D$36:$D$41</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Plan1!$F$36:$F$41</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>89600</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>193536</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>891000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1430000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2676960</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7603200</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="233504768"/>
+        <c:axId val="233510368"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="233504768"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="233510368"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="233510368"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="233504768"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
@@ -969,8 +1917,1059 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="290">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk2">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="31750" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700">
+        <a:solidFill>
+          <a:schemeClr val="lt2"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -1499,6 +3498,66 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>157162</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>147637</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1376362</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>33337</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Gráfico 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>138112</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>119062</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1357312</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>4762</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Gráfico 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1770,10 +3829,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:G33"/>
+  <dimension ref="A3:G41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="G30" sqref="G30"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2152,6 +4211,83 @@
         <v>20.482931300000001</v>
       </c>
     </row>
+    <row r="35" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D35" t="s">
+        <v>8</v>
+      </c>
+      <c r="E35" t="s">
+        <v>12</v>
+      </c>
+      <c r="F35" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="36" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D36">
+        <v>50</v>
+      </c>
+      <c r="E36">
+        <v>327680</v>
+      </c>
+      <c r="F36">
+        <v>89600</v>
+      </c>
+    </row>
+    <row r="37" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D37">
+        <v>60</v>
+      </c>
+      <c r="E37">
+        <v>990000</v>
+      </c>
+      <c r="F37">
+        <v>193536</v>
+      </c>
+    </row>
+    <row r="38" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D38">
+        <v>70</v>
+      </c>
+      <c r="E38">
+        <v>2488320</v>
+      </c>
+      <c r="F38">
+        <v>891000</v>
+      </c>
+    </row>
+    <row r="39" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D39">
+        <v>80</v>
+      </c>
+      <c r="E39">
+        <v>5493488</v>
+      </c>
+      <c r="F39">
+        <v>1430000</v>
+      </c>
+    </row>
+    <row r="40" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D40">
+        <v>90</v>
+      </c>
+      <c r="E40">
+        <v>11010048</v>
+      </c>
+      <c r="F40">
+        <v>2676960</v>
+      </c>
+    </row>
+    <row r="41" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D41">
+        <v>100</v>
+      </c>
+      <c r="E41">
+        <v>20470320</v>
+      </c>
+      <c r="F41">
+        <v>7603200</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
update on the charts - excel
</commit_message>
<xml_diff>
--- a/Algorithm/Test results/tests version 3.xlsx
+++ b/Algorithm/Test results/tests version 3.xlsx
@@ -150,7 +150,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx2"/>
                 </a:solidFill>
@@ -160,7 +160,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="fr-FR"/>
+              <a:rPr lang="fr-FR" b="0"/>
               <a:t>Experiment 1</a:t>
             </a:r>
           </a:p>
@@ -180,7 +180,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx2"/>
               </a:solidFill>
@@ -734,12 +734,12 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="208936944"/>
-        <c:axId val="208937504"/>
+        <c:axId val="220272672"/>
+        <c:axId val="220273232"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="208936944"/>
+        <c:axId val="220272672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -762,7 +762,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="fr-FR"/>
+                  <a:rPr lang="fr-FR" b="0"/>
                   <a:t>Number of concrete services</a:t>
                 </a:r>
               </a:p>
@@ -829,7 +829,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="208937504"/>
+        <c:crossAx val="220273232"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -837,7 +837,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="208937504"/>
+        <c:axId val="220273232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -874,8 +874,8 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="fr-FR"/>
-                  <a:t>Time</a:t>
+                  <a:rPr lang="fr-FR" b="0"/>
+                  <a:t>Processing time</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -935,7 +935,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="208936944"/>
+        <c:crossAx val="220272672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -948,7 +948,7 @@
       </c:spPr>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="b"/>
+      <c:legendPos val="r"/>
       <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
@@ -1008,7 +1008,7 @@
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-    <c:pageSetup/>
+    <c:pageSetup orientation="portrait"/>
   </c:printSettings>
 </c:chartSpace>
 </file>
@@ -1258,16 +1258,77 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="230883968"/>
-        <c:axId val="226168512"/>
+        <c:axId val="124471600"/>
+        <c:axId val="124469920"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="230883968"/>
+        <c:axId val="124471600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="fr-FR"/>
+                  <a:t>Number of concrete</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="fr-FR" baseline="0"/>
+                  <a:t> services</a:t>
+                </a:r>
+                <a:endParaRPr lang="fr-FR"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="fr-FR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1305,7 +1366,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="226168512"/>
+        <c:crossAx val="124469920"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1313,7 +1374,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="226168512"/>
+        <c:axId val="124469920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1333,6 +1394,62 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="fr-FR"/>
+                  <a:t>Porcessing  time</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="fr-FR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1364,7 +1481,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="230883968"/>
+        <c:crossAx val="124471600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1377,7 +1494,7 @@
       </c:spPr>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="b"/>
+      <c:legendPos val="r"/>
       <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
@@ -1440,7 +1557,7 @@
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-    <c:pageSetup/>
+    <c:pageSetup orientation="portrait"/>
   </c:printSettings>
 </c:chartSpace>
 </file>
@@ -1480,7 +1597,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="fr-FR"/>
-              <a:t>Experiment 3</a:t>
+              <a:t>Experiment 2</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -1690,16 +1807,72 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="233504768"/>
-        <c:axId val="233510368"/>
+        <c:axId val="252973216"/>
+        <c:axId val="252973776"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="233504768"/>
+        <c:axId val="252973216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="fr-FR"/>
+                  <a:t>Number of concrete services</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="fr-FR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1737,7 +1910,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="233510368"/>
+        <c:crossAx val="252973776"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1745,7 +1918,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="233510368"/>
+        <c:axId val="252973776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1765,6 +1938,62 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="fr-FR"/>
+                  <a:t>Number of rewritings</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="fr-FR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1796,7 +2025,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="233504768"/>
+        <c:crossAx val="252973216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1809,7 +2038,7 @@
       </c:spPr>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="b"/>
+      <c:legendPos val="r"/>
       <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
@@ -1872,7 +2101,7 @@
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-    <c:pageSetup/>
+    <c:pageSetup orientation="portrait"/>
   </c:printSettings>
 </c:chartSpace>
 </file>
@@ -3831,8 +4060,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:G41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4290,7 +4519,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="95" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
VLDB paper: approach and conclusions
</commit_message>
<xml_diff>
--- a/Algorithm/Test results/tests version 3.xlsx
+++ b/Algorithm/Test results/tests version 3.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7935"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7935" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
+    <sheet name="Plan2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="16">
   <si>
     <t xml:space="preserve">Testcase: 0 </t>
   </si>
@@ -66,6 +67,12 @@
   </si>
   <si>
     <t>Test 2</t>
+  </si>
+  <si>
+    <t>Traditional approach</t>
+  </si>
+  <si>
+    <t>Preferences-guided approach</t>
   </si>
 </sst>
 </file>
@@ -734,12 +741,12 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="220272672"/>
-        <c:axId val="220273232"/>
+        <c:axId val="114325712"/>
+        <c:axId val="114326272"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="220272672"/>
+        <c:axId val="114325712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -829,7 +836,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="220273232"/>
+        <c:crossAx val="114326272"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -837,7 +844,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="220273232"/>
+        <c:axId val="114326272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -935,7 +942,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="220272672"/>
+        <c:crossAx val="114325712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1258,11 +1265,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="124471600"/>
-        <c:axId val="124469920"/>
+        <c:axId val="114329632"/>
+        <c:axId val="114330192"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="124471600"/>
+        <c:axId val="114329632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1366,7 +1373,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="124469920"/>
+        <c:crossAx val="114330192"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1374,7 +1381,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="124469920"/>
+        <c:axId val="114330192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1481,7 +1488,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="124471600"/>
+        <c:crossAx val="114329632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1807,11 +1814,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="252973216"/>
-        <c:axId val="252973776"/>
+        <c:axId val="204887088"/>
+        <c:axId val="204887648"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="252973216"/>
+        <c:axId val="204887088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1910,7 +1917,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="252973776"/>
+        <c:crossAx val="204887648"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1918,7 +1925,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="252973776"/>
+        <c:axId val="204887648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2025,7 +2032,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="252973216"/>
+        <c:crossAx val="204887088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2102,6 +2109,1112 @@
     <c:headerFooter/>
     <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
     <c:pageSetup orientation="portrait"/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="pt-BR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="fr-FR"/>
+              <a:t>Performance</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Plan2!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Traditional approach</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Plan2!$A$2:$A$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Plan2!$B$2:$B$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.42120269999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.73320470000000004</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.8252117000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.8252117000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9.6564619</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>15.163297200000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Plan2!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Preferences-guided approach</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Plan2!$A$2:$A$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Plan2!$C$2:$C$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.17160110000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.18720120000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.70200450000000003</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.0920069999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.9812126999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.5224354</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="206629168"/>
+        <c:axId val="206628608"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="206629168"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="fr-FR"/>
+                  <a:t>Number of concrete</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="fr-FR" baseline="0"/>
+                  <a:t> services</a:t>
+                </a:r>
+                <a:endParaRPr lang="fr-FR"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="fr-FR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="206628608"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="206628608"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="fr-FR"/>
+                  <a:t>Time in seconds</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="fr-FR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="206629168"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="fr-FR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+    <c:pageSetup paperSize="9" orientation="landscape"/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="pt-BR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="fr-FR"/>
+              <a:t>Integration cost</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Plan2!$B$9</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Traditional approach</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Plan2!$A$10:$A$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Plan2!$B$10:$B$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>196608</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>594000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1492992</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3296092.8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6606028.7999999998</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>12282192</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Plan2!$C$9</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Preferences-guided approach</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Plan2!$A$10:$A$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Plan2!$C$10:$C$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>53760</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>116121.59999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>891000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>858000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1606176</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4561920</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="259493904"/>
+        <c:axId val="259495024"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="259493904"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="fr-FR"/>
+                  <a:t>Number of</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="fr-FR" baseline="0"/>
+                  <a:t> concrete services</a:t>
+                </a:r>
+                <a:endParaRPr lang="fr-FR"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="fr-FR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="259495024"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="259495024"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="fr-FR"/>
+                  <a:t>Number of rewritings</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="fr-FR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="259493904"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="fr-FR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+    <c:pageSetup paperSize="9" orientation="landscape"/>
   </c:printSettings>
 </c:chartSpace>
 </file>
@@ -2226,6 +3339,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="290">
   <cs:axisTitle>
@@ -3347,6 +4540,1038 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -3787,6 +6012,71 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>4762</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>390525</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>80962</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Gráfico 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>100012</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>176212</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Gráfico 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -4060,8 +6350,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:G41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="F41" sqref="E36:F41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4522,4 +6812,190 @@
   <pageSetup paperSize="9" scale="95" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>50</v>
+      </c>
+      <c r="B2">
+        <v>0.42120269999999999</v>
+      </c>
+      <c r="C2">
+        <v>0.17160110000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>60</v>
+      </c>
+      <c r="B3">
+        <v>0.73320470000000004</v>
+      </c>
+      <c r="C3">
+        <v>0.18720120000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>70</v>
+      </c>
+      <c r="B4">
+        <v>1.8252117000000001</v>
+      </c>
+      <c r="C4">
+        <v>0.70200450000000003</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>80</v>
+      </c>
+      <c r="B5">
+        <v>1.8252117000000001</v>
+      </c>
+      <c r="C5">
+        <v>1.0920069999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>90</v>
+      </c>
+      <c r="B6">
+        <v>9.6564619</v>
+      </c>
+      <c r="C6">
+        <v>1.9812126999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>100</v>
+      </c>
+      <c r="B7">
+        <v>15.163297200000001</v>
+      </c>
+      <c r="C7">
+        <v>5.5224354</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>50</v>
+      </c>
+      <c r="B10">
+        <f>327680*0.6</f>
+        <v>196608</v>
+      </c>
+      <c r="C10">
+        <f>89600*0.6</f>
+        <v>53760</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>60</v>
+      </c>
+      <c r="B11">
+        <f>990000*0.6</f>
+        <v>594000</v>
+      </c>
+      <c r="C11">
+        <f>193536*0.6</f>
+        <v>116121.59999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>70</v>
+      </c>
+      <c r="B12">
+        <f>2488320*0.6</f>
+        <v>1492992</v>
+      </c>
+      <c r="C12">
+        <v>891000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>80</v>
+      </c>
+      <c r="B13">
+        <f>5493488*0.6</f>
+        <v>3296092.8</v>
+      </c>
+      <c r="C13">
+        <f>1430000*0.6</f>
+        <v>858000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>90</v>
+      </c>
+      <c r="B14">
+        <f>11010048*0.6</f>
+        <v>6606028.7999999998</v>
+      </c>
+      <c r="C14">
+        <f>2676960*0.6</f>
+        <v>1606176</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>100</v>
+      </c>
+      <c r="B15">
+        <f>20470320*0.6</f>
+        <v>12282192</v>
+      </c>
+      <c r="C15">
+        <f>7603200*0.6</f>
+        <v>4561920</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>